<commit_message>
Push broke yesterday so here's everything from 2 days
FBX files can be loaded
Tried to do animation but got stuck and couldn't figure out the last big so gave up
Added Capsule to box collision
Added player death
Added textures to particles
Added transparency to particles and text
Added really awful "sprite" animation with OBJ files
Made particles trigger on things happening
</commit_message>
<xml_diff>
--- a/Assignment 2 checklist.xlsx
+++ b/Assignment 2 checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\AGP-Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{49C4338A-16B4-4B52-87DD-F399C3453732}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{77963C31-7EB2-4F81-AAC2-2F0A25F56A32}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28125" windowHeight="9705" xr2:uid="{55536DC3-F3A6-4901-8C52-0177ACD9FD83}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="126">
   <si>
     <t>Report</t>
   </si>
@@ -417,6 +417,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>FBX loading</t>
+  </si>
+  <si>
+    <t>Component System</t>
   </si>
 </sst>
 </file>
@@ -483,17 +489,132 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -803,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5441D33C-E496-40B9-9987-72D769C4F1A0}">
-  <dimension ref="A1:B131"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,19 +936,23 @@
     <col min="7" max="7" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>SUM(B3:B5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -835,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -843,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -851,13 +976,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>SUM(B7:B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -865,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -873,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -881,13 +1010,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>SUM(B11:B13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -895,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -903,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -911,19 +1044,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15">
+        <f>SUM(B16:B18)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -931,7 +1068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -939,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -947,13 +1084,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f>SUM(B20:B22)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -961,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -969,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -977,13 +1118,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f>SUM(B24:B25)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -991,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -999,13 +1144,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f>SUM(B27:B28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1013,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1021,13 +1170,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f>SUM(B30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1035,13 +1188,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f>SUM(B32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1049,13 +1206,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="63.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A33" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+      <c r="C33">
+        <f>SUM(B34:B36)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1063,7 +1224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1071,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1079,13 +1240,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f>SUM(B38:B39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1093,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1101,19 +1266,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="5"/>
-    </row>
-    <row r="41" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <f>SUM(B42:B44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
@@ -1121,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
@@ -1129,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>55</v>
       </c>
@@ -1137,13 +1306,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B45" s="4"/>
-    </row>
-    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f>SUM(B46:B48)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>57</v>
       </c>
@@ -1151,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>58</v>
       </c>
@@ -1159,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>59</v>
       </c>
@@ -1167,13 +1340,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B49" s="4"/>
-    </row>
-    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <f>SUM(B50:B52)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>61</v>
       </c>
@@ -1181,7 +1358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
@@ -1189,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>63</v>
       </c>
@@ -1197,19 +1374,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A53" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B53" s="5"/>
     </row>
-    <row r="54" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B54" s="4"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <f>SUM(B55:B57)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
@@ -1217,15 +1398,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>43</v>
       </c>
@@ -1233,21 +1414,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A58" s="7" t="s">
+    <row r="58" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A58" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="7"/>
-    </row>
-    <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="6"/>
+      <c r="C58">
+        <f>SUM(B59:B61)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>46</v>
       </c>
@@ -1255,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>47</v>
       </c>
@@ -1263,13 +1448,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B62" s="4"/>
-    </row>
-    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <f>SUM(B63:B65)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>49</v>
       </c>
@@ -1277,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>50</v>
       </c>
@@ -1285,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>51</v>
       </c>
@@ -1293,19 +1482,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A66" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B66" s="5"/>
     </row>
-    <row r="67" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B67" s="4"/>
-    </row>
-    <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <f>SUM(B68:B70)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -1313,7 +1506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -1321,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -1329,13 +1522,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B71" s="4"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <f>SUM(B72:B74)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -1343,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -1351,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -1359,13 +1556,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B75" s="4"/>
-    </row>
-    <row r="76" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <f>SUM(B76:B78)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>49</v>
       </c>
@@ -1373,7 +1574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>50</v>
       </c>
@@ -1381,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>51</v>
       </c>
@@ -1389,19 +1590,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A79" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B79" s="5"/>
     </row>
-    <row r="80" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B80" s="4"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <f>SUM(B81:B82)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>77</v>
       </c>
@@ -1409,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>78</v>
       </c>
@@ -1417,13 +1622,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>79</v>
       </c>
       <c r="B83" s="4"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <f>SUM(B84:B85)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -1431,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -1439,13 +1648,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B86" s="4"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <f>SUM(B87:B89)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>83</v>
       </c>
@@ -1453,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>84</v>
       </c>
@@ -1461,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -1469,13 +1682,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B90" s="4"/>
-    </row>
-    <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <f>SUM(B91:B93)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>87</v>
       </c>
@@ -1483,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>89</v>
       </c>
@@ -1491,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>88</v>
       </c>
@@ -1499,13 +1716,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B94" s="4"/>
-    </row>
-    <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <f>SUM(B95:B97)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>91</v>
       </c>
@@ -1513,7 +1734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>92</v>
       </c>
@@ -1521,21 +1742,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B98" s="4"/>
-    </row>
-    <row r="99" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <f>SUM(B99:B100)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>95</v>
       </c>
@@ -1543,27 +1768,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A101" s="5" t="s">
         <v>97</v>
       </c>
       <c r="B101" s="5"/>
     </row>
-    <row r="102" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B102" s="4"/>
-    </row>
-    <row r="103" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <f>SUM(B103:B105)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>99</v>
       </c>
@@ -1571,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>100</v>
       </c>
@@ -1579,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>101</v>
       </c>
@@ -1587,13 +1816,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B106" s="4"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <f>SUM(B107:B109)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>103</v>
       </c>
@@ -1601,7 +1834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>104</v>
       </c>
@@ -1609,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>105</v>
       </c>
@@ -1617,13 +1850,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>106</v>
       </c>
       <c r="B110" s="4"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <f>SUM(B111:B116)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>107</v>
       </c>
@@ -1631,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>108</v>
       </c>
@@ -1639,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>109</v>
       </c>
@@ -1647,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>110</v>
       </c>
@@ -1655,7 +1892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>111</v>
       </c>
@@ -1663,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>112</v>
       </c>
@@ -1671,13 +1908,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B117" s="4"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <f>SUM(B118:B121)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>114</v>
       </c>
@@ -1685,15 +1926,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>116</v>
       </c>
@@ -1701,7 +1942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>117</v>
       </c>
@@ -1709,13 +1950,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>118</v>
       </c>
       <c r="B122" s="4"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <f>SUM(B123:B125)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -1723,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -1731,7 +1976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>121</v>
       </c>
@@ -1739,20 +1984,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B126" s="4"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <f>SUM(B127:B129)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>124</v>
+      </c>
       <c r="B127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>125</v>
+      </c>
       <c r="B128">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -1766,30 +2021,18 @@
       </c>
       <c r="B131">
         <f>SUM(B3:B5,B7:B9,B11:B13,B16:B18,B20:B22,B24:B25,B27:B28,B30,B32,B34:B36,B38:B39,B42:B44,B46:B48,B50:B52,B55:B57,B59:B61,B63:B65,B68:B70,B72:B74,B76:B78,B81:B82,B84:B85,B87:B89,B91:B93,B95:B97,B99:B100,B103:B105,B107:B109,B111:B116,B118:B121,B123:B125,B127:B129)</f>
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A122:B122"/>
     <mergeCell ref="A98:B98"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A66:B66"/>
@@ -1803,14 +2046,56 @@
     <mergeCell ref="A86:B86"/>
     <mergeCell ref="A90:B90"/>
     <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
+  <conditionalFormatting sqref="A2:B2">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$C$2&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B5 B7:B9 B11:B13 B16:B18 B20:B22 B24:B25 B27:B28 B30 B32 B34:B36 B38:B39 B42:B44 B46:B48 B50:B52 B55:B57 B59:B61 B63:B65 B68:B70 B72:B74 B76:B78 B81:B82 B84:B85 B87:B89 B91:B93 B95:B97 B99:B100 B103:B105 B107:B109 B111:B116 B118:B121 B123:B125 B127:B129">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B124:B125">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B124:B125">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>